<commit_message>
yeni dosyada ilk degisiklik
</commit_message>
<xml_diff>
--- a/yonetim.xlsx
+++ b/yonetim.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="1">
   <si>
     <t>sure</t>
   </si>
@@ -370,7 +370,7 @@
   <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B19"/>
+      <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -379,19 +379,45 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" s="1">

</xml_diff>